<commit_message>
EPBDS-6528 Replace myType.getAmount() with myType.amount
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test-resources/functionality/NullSafetyOperations.xlsx
+++ b/DEV/org.openl.test/test-resources/functionality/NullSafetyOperations.xlsx
@@ -66,12 +66,6 @@
     <t>NullType</t>
   </si>
   <si>
-    <t>=type.getAmount()</t>
-  </si>
-  <si>
-    <t>=$s1.getAmount()</t>
-  </si>
-  <si>
     <t>= NullSafety(null)</t>
   </si>
   <si>
@@ -214,6 +208,12 @@
   </si>
   <si>
     <t>=isEmpty(removeNulls($case3))</t>
+  </si>
+  <si>
+    <t>=type.amount</t>
+  </si>
+  <si>
+    <t>=$s1.amount</t>
   </si>
 </sst>
 </file>
@@ -360,12 +360,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -377,6 +371,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -386,17 +388,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1 10" xfId="9"/>
@@ -710,7 +710,7 @@
   <dimension ref="C5:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,295 +723,295 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="H5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="H9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="H13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="8"/>
+      <c r="H14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="8"/>
+      <c r="H15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="9"/>
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="H5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="17" t="s">
+      <c r="K16" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="H17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="H18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="H19" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="H13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="13"/>
-      <c r="H14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="13"/>
-      <c r="H15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="14"/>
-      <c r="H16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="8" t="s">
+      <c r="I19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="H20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K16" s="8" t="s">
+      <c r="I20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="H24" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="H17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="H18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="H19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="H20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J32" s="9" t="b">
+        <v>55</v>
+      </c>
+      <c r="J32" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J33" t="b">
         <v>1</v>
@@ -1019,21 +1019,21 @@
     </row>
     <row r="34" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J35" t="b">
         <v>1</v>
@@ -1041,10 +1041,10 @@
     </row>
     <row r="36" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J36" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
EPBDS-6819 Null-safety doesn't work for Spreadsheets
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test-resources/functionality/NullSafetyOperations.xlsx
+++ b/DEV/org.openl.test/test-resources/functionality/NullSafetyOperations.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24915" windowHeight="12585"/>
+    <workbookView windowHeight="12585" windowWidth="24915" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Datatypes" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -214,19 +218,64 @@
   </si>
   <si>
     <t>=$s1.amount</t>
+  </si>
+  <si>
+    <t>case5</t>
+  </si>
+  <si>
+    <t>= false ? NullSafety(new MyType[] {null, null}) : null</t>
+  </si>
+  <si>
+    <t>case6</t>
+  </si>
+  <si>
+    <t>= $case5.$NullCell$Value</t>
+  </si>
+  <si>
+    <t>= $case5</t>
+  </si>
+  <si>
+    <t>= false ? NullSafety(null) : null</t>
+  </si>
+  <si>
+    <t>= $case5.$Value$NullCell</t>
+  </si>
+  <si>
+    <t>_res_.$ArgNull$case5</t>
+  </si>
+  <si>
+    <t>_res_.$ArgNull$case6</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>_res_.$ConstNul$case5</t>
+  </si>
+  <si>
+    <t>_res_.$ConstNul$case6</t>
+  </si>
+  <si>
+    <t>_res_.$ConstNull$case5</t>
+  </si>
+  <si>
+    <t>_res_.$ConstNull$case6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="000000" theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -274,12 +323,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="1F497D" theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -343,92 +398,63 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="13">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
-    <cellStyle name="20% - Accent1 10" xfId="9"/>
-    <cellStyle name="20% - Accent1 2" xfId="2"/>
-    <cellStyle name="20% - Accent1 3" xfId="3"/>
-    <cellStyle name="20% - Accent1 5" xfId="4"/>
-    <cellStyle name="20% - Accent3 10" xfId="5"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 5" xfId="6"/>
-    <cellStyle name="Обычный 5 3" xfId="7"/>
-    <cellStyle name="Обычный 6" xfId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="20% - Accent1 10" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -461,9 +487,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,9 +522,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,9 +574,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,7 +646,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -595,13 +655,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -611,7 +671,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -620,7 +680,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -629,7 +689,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -639,12 +699,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -675,7 +735,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -694,7 +754,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -706,382 +766,402 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:K36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="H5" s="17" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="10" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="10" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H9" s="10" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="C9" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="H13" s="12" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="14"/>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8"/>
-      <c r="H14" s="1" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="8"/>
-      <c r="H15" s="1" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="9"/>
-      <c r="H16" s="1" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="H17" s="1" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="H18" s="1" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="H19" s="1" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="5"/>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="H20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="15" t="s">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I25" t="s">
+      <c r="C26" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H26" t="s">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I26" t="s">
+      <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J26" t="s">
+      <c r="D27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H27" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I27" t="s">
+      <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H28" t="s">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I28" t="s">
+      <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H29" t="s">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I29" t="s">
+      <c r="C30" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H30" t="s">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I30" t="s">
+      <c r="C31" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H31" t="s">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I31" t="s">
+      <c r="C32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J31" t="s">
+      <c r="D32" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H32" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I32" t="s">
+      <c r="C33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J32" s="7" t="b">
+      <c r="D33" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H33" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I33" t="s">
+      <c r="C34" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J33" t="b">
+      <c r="D34" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H34" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I34" t="s">
+      <c r="C35" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J34" t="s">
+      <c r="D35" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H35" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I35" t="s">
+      <c r="C36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J35" t="b">
+      <c r="D36" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H36" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I36" t="s">
+      <c r="C37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J36" t="b">
+      <c r="D37" s="1" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="38">
+      <c r="B38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="H5:I5"/>
+  <mergeCells count="3">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row ht="30" r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>